<commit_message>
Added a credits scene and credits roll animation
</commit_message>
<xml_diff>
--- a/Assets/Audio/Silent Space Audio Asset List.xlsx
+++ b/Assets/Audio/Silent Space Audio Asset List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/Assets/Audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04438A8A-A273-C34B-8607-C6BB605791FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4072C6BD-4799-404E-B425-314B9F80C22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51560" yWindow="7700" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52620" yWindow="7700" windowWidth="36980" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SFX" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="269">
   <si>
     <t>Sound Effect Asset List</t>
   </si>
@@ -455,21 +455,12 @@
     <t>Player: Weapons</t>
   </si>
   <si>
-    <t>Environment: Fungus</t>
-  </si>
-  <si>
     <t>Environment: Ambience</t>
   </si>
   <si>
-    <t>Trigger Collider Prefab</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
-    <t>Environment: Security</t>
-  </si>
-  <si>
     <t>Gravity Room Ambience</t>
   </si>
   <si>
@@ -485,9 +476,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Gravity Room</t>
-  </si>
-  <si>
     <t>Base Ambience</t>
   </si>
   <si>
@@ -500,9 +488,6 @@
     <t>sfx_ui_pause.wav</t>
   </si>
   <si>
-    <t>sfx_ambience_base</t>
-  </si>
-  <si>
     <t>Safe Room</t>
   </si>
   <si>
@@ -512,28 +497,355 @@
     <t>sfx_ambience_safe</t>
   </si>
   <si>
-    <t>sfx_ambience_gravity</t>
-  </si>
-  <si>
-    <t>Low Gravity Room Ambience</t>
-  </si>
-  <si>
-    <t>Scrapyard Ambience</t>
-  </si>
-  <si>
-    <t>sfx_ambience_scrapyard</t>
-  </si>
-  <si>
     <t>sfx_ambience_boss</t>
   </si>
   <si>
-    <t>Misc. Rooms</t>
-  </si>
-  <si>
-    <t>Scrapyard</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - IMPLEMENTED</t>
+  </si>
+  <si>
+    <t>Screamer Screeching Sequence</t>
+  </si>
+  <si>
+    <t>Player Running (Glass)</t>
+  </si>
+  <si>
+    <t>Player Running (Flesh)</t>
+  </si>
+  <si>
+    <t>Player Running (Wood)</t>
+  </si>
+  <si>
+    <t>Player Hurt</t>
+  </si>
+  <si>
+    <t>sfx_player_stun_fire</t>
+  </si>
+  <si>
+    <t>sfx_player_stun_upgrade_#</t>
+  </si>
+  <si>
+    <t>sfx_player_stun_cooldown</t>
+  </si>
+  <si>
+    <t>sfx_player_emp</t>
+  </si>
+  <si>
+    <t>sfx_player_grenade_fire</t>
+  </si>
+  <si>
+    <t>sfx_player_grenade_freeze</t>
+  </si>
+  <si>
+    <t>sfx_player_grenade_upgrade_#</t>
+  </si>
+  <si>
+    <t>sfx_player_lethal_gun_fire</t>
+  </si>
+  <si>
+    <t>Lethal Gun Fire</t>
+  </si>
+  <si>
+    <t>Stun Gun Cooldown Complete</t>
+  </si>
+  <si>
+    <t>sfx_player_stun_cooldown_complete</t>
+  </si>
+  <si>
+    <t>sfx_player_suit_upgrade</t>
+  </si>
+  <si>
+    <t>sfx_player_jetpack_dash</t>
+  </si>
+  <si>
+    <t>sfx_player_jetpack_upgrade_#</t>
+  </si>
+  <si>
+    <t>sfx_player_jetpack_fuel_meter</t>
+  </si>
+  <si>
+    <t>sfx_player_jetpack_fuel_ultimate</t>
+  </si>
+  <si>
+    <t>sfx_player_footsteps_metal_#</t>
+  </si>
+  <si>
+    <t>sfx_player_footsteps_glass_#</t>
+  </si>
+  <si>
+    <t>sfx_player_footsteps_flesh_#</t>
+  </si>
+  <si>
+    <t>sfx_player_footsteps_wood_#</t>
+  </si>
+  <si>
+    <t>sfx_player_jump</t>
+  </si>
+  <si>
+    <t>sfx_player_hurt_#</t>
+  </si>
+  <si>
+    <t>sfx_player_health_replenish</t>
+  </si>
+  <si>
+    <t>Noise Meter Trigger 1-3</t>
+  </si>
+  <si>
+    <t>sfx_noise_meter_trigger_#</t>
+  </si>
+  <si>
+    <t>sfx_noise_meter_tentacle_element</t>
+  </si>
+  <si>
+    <t>sfx_player_instant_kill</t>
+  </si>
+  <si>
+    <t>sfx_enemie_tentacle_spawn</t>
+  </si>
+  <si>
+    <t>sfx_enemie_tentacle_ambience</t>
+  </si>
+  <si>
+    <t>sfx_enemie_infected_idle</t>
+  </si>
+  <si>
+    <t>Infected Hurt</t>
+  </si>
+  <si>
+    <t>sfx_enemie_infected_hurt_#</t>
+  </si>
+  <si>
+    <t>sfx_enemie_infected_attacking_#</t>
+  </si>
+  <si>
+    <t>sfx_enemie_infected_death_#</t>
+  </si>
+  <si>
+    <t>sfx_enemie_crawlers_explode</t>
+  </si>
+  <si>
+    <t>sfx_enemie_crawlers_attacking</t>
+  </si>
+  <si>
+    <t>sfx_enemie_crawlers_hurt</t>
+  </si>
+  <si>
+    <t>Crawlers Hurt</t>
+  </si>
+  <si>
+    <t>sfx_enemie_crawlers_idle</t>
+  </si>
+  <si>
+    <t>sfx_enemie_screamer_idle</t>
+  </si>
+  <si>
+    <t>sfx_enemie_screamer_screaching</t>
+  </si>
+  <si>
+    <t>sfx_enemie_screamer_death</t>
+  </si>
+  <si>
+    <t>sfx_enemie_glob_idle</t>
+  </si>
+  <si>
+    <t>sfx_enemie_glob_death</t>
+  </si>
+  <si>
+    <t>sfx_enemie_glob_attacking</t>
+  </si>
+  <si>
+    <t>Glob Alerted?</t>
+  </si>
+  <si>
+    <t>jellyfish like creatures</t>
+  </si>
+  <si>
+    <t>overinfected but weak vessle of flesh</t>
+  </si>
+  <si>
+    <t>infected like spiders</t>
+  </si>
+  <si>
+    <t>infected crew members</t>
+  </si>
+  <si>
+    <t>tentacles</t>
+  </si>
+  <si>
+    <t>giant overgrown infected blob</t>
+  </si>
+  <si>
+    <t>sfx_enemie_liptank_idle</t>
+  </si>
+  <si>
+    <t>sfx_enemie_liptank_attacking</t>
+  </si>
+  <si>
+    <t>sfx_enemie_liptank_death</t>
+  </si>
+  <si>
+    <t>Xeno-encephalon Attacking Through Ceiling &amp; Floor</t>
+  </si>
+  <si>
+    <t>Xeno-encephalon Gas Attack</t>
+  </si>
+  <si>
+    <t>Xeno-encephalon Head Slam</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_idle</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_death_sequence</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_damaged</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_head_slam</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_gas_attack</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_attack_through_surface</t>
+  </si>
+  <si>
+    <t>sfx_enemie_xeno-encephalon_movement</t>
+  </si>
+  <si>
+    <t>boss of the game - two skeleton heads with a brain for a body</t>
+  </si>
+  <si>
+    <t>sfx_enemie_eye_stalker_death</t>
+  </si>
+  <si>
+    <t>sfx_enemie_eye_stalker_alerted</t>
+  </si>
+  <si>
+    <t>sfx_enemie_eye_stalker_idle</t>
+  </si>
+  <si>
+    <t>sfx_environment_fungus_destoryed</t>
+  </si>
+  <si>
+    <t>sfx_environment_fungus_ambience</t>
+  </si>
+  <si>
+    <t>sfx_environment_security_alarm_activated</t>
+  </si>
+  <si>
+    <t>small eye of xeno-encephalon that follows the player and increases the noise meter</t>
+  </si>
+  <si>
+    <t>sfx_objects_alien_artifact_#</t>
+  </si>
+  <si>
+    <t>sfx_objects_audio_log_activation</t>
+  </si>
+  <si>
+    <t>increases noise meter</t>
+  </si>
+  <si>
+    <t>blocks player's path</t>
+  </si>
+  <si>
+    <t>Infected Attacking</t>
+  </si>
+  <si>
+    <t>0 Gravity Room</t>
+  </si>
+  <si>
+    <t>Hallways</t>
+  </si>
+  <si>
+    <t>Med Bay</t>
+  </si>
+  <si>
+    <t>Med Bay Ambience</t>
+  </si>
+  <si>
+    <t>sfx_ambience_med_bay</t>
+  </si>
+  <si>
+    <t>Hallway Ambience</t>
+  </si>
+  <si>
+    <t>sfx_ambience_hallway</t>
+  </si>
+  <si>
+    <t>Bridge Ambience</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Escape Pod Hatch</t>
+  </si>
+  <si>
+    <t>Escape Pod Hatch Ambience</t>
+  </si>
+  <si>
+    <t>sfx_ambience_escape_pod_hatch</t>
+  </si>
+  <si>
+    <t>Ship Hull Ambience</t>
+  </si>
+  <si>
+    <t>Room that holds constellation keys</t>
+  </si>
+  <si>
+    <t>Alien monologues are used in this area</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Warehouse Ambience</t>
+  </si>
+  <si>
+    <t>Origin of infection spreading</t>
+  </si>
+  <si>
+    <t>where the infected alien artifact was found</t>
+  </si>
+  <si>
+    <t>General Areas</t>
+  </si>
+  <si>
+    <t>sfx_ambience_ship_hull</t>
+  </si>
+  <si>
+    <t>sfx_ambience_warehouse</t>
+  </si>
+  <si>
+    <t>sfx_ambience_general</t>
+  </si>
+  <si>
+    <t>Voice Log Activation (6)</t>
+  </si>
+  <si>
+    <t>Environment:</t>
+  </si>
+  <si>
+    <t>Elevator</t>
+  </si>
+  <si>
+    <t>Elevator Movement</t>
+  </si>
+  <si>
+    <t>sfx_environment_elevator</t>
+  </si>
+  <si>
+    <t>A general track for ambience in other non key areas</t>
+  </si>
+  <si>
+    <t>Ship Hull</t>
+  </si>
+  <si>
+    <t>When the noise meter reaches 100% the player will get insta killed</t>
+  </si>
+  <si>
+    <t>Step Playlist Container</t>
   </si>
 </sst>
 </file>
@@ -855,8 +1167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="C3:J67" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="C3:J67" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="C3:J73" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="C3:J73" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="STATUS" dataDxfId="3" dataCellStyle="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="LOCATION"/>
@@ -1209,10 +1521,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1223,8 +1535,9 @@
     <col min="4" max="5" width="28.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
     <col min="7" max="7" width="40.83203125" customWidth="1"/>
-    <col min="8" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="38.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.5" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="29.83203125" customWidth="1"/>
     <col min="13" max="13" width="34.83203125" customWidth="1"/>
@@ -1243,7 +1556,7 @@
     </row>
     <row r="3" spans="1:14" ht="22.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1289,16 +1602,19 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="15"/>
       <c r="D4" t="s">
         <v>74</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="I4" t="s">
+        <v>159</v>
+      </c>
       <c r="K4" s="16"/>
       <c r="L4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M4" t="s">
         <v>15</v>
@@ -1318,6 +1634,12 @@
       <c r="E5" t="s">
         <v>61</v>
       </c>
+      <c r="H5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I5" t="s">
+        <v>160</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" t="s">
         <v>3</v>
@@ -1333,12 +1655,15 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="15"/>
       <c r="D6" t="s">
         <v>74</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>161</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" t="s">
@@ -1355,12 +1680,18 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="15"/>
       <c r="D7" t="s">
         <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>168</v>
+      </c>
+      <c r="H7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I7" t="s">
+        <v>169</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" t="s">
@@ -1382,7 +1713,10 @@
         <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
       </c>
       <c r="M8" t="s">
         <v>65</v>
@@ -1395,12 +1729,15 @@
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="15"/>
       <c r="D9" t="s">
         <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>163</v>
       </c>
       <c r="M9" t="s">
         <v>60</v>
@@ -1413,12 +1750,15 @@
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="15"/>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="I10" t="s">
+        <v>164</v>
       </c>
       <c r="M10" t="s">
         <v>59</v>
@@ -1436,7 +1776,13 @@
         <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>268</v>
+      </c>
+      <c r="I11" t="s">
+        <v>165</v>
       </c>
       <c r="K11" s="11"/>
       <c r="M11" t="s">
@@ -1447,18 +1793,18 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>124</v>
-      </c>
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="15"/>
       <c r="D12" t="s">
         <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>167</v>
+      </c>
+      <c r="I12" t="s">
+        <v>166</v>
       </c>
       <c r="K12" s="11"/>
       <c r="M12" t="s">
@@ -1469,6 +1815,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
       <c r="B13">
         <v>10</v>
       </c>
@@ -1477,7 +1826,13 @@
         <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>268</v>
+      </c>
+      <c r="I13" t="s">
+        <v>170</v>
       </c>
       <c r="K13" s="11"/>
       <c r="M13" t="s">
@@ -1491,12 +1846,15 @@
       <c r="B14">
         <v>11</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="15"/>
       <c r="D14" t="s">
         <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>171</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1514,7 +1872,13 @@
         <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="H15" t="s">
+        <v>268</v>
+      </c>
+      <c r="I15" t="s">
+        <v>172</v>
       </c>
       <c r="M15" t="s">
         <v>63</v>
@@ -1532,7 +1896,13 @@
         <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="H16" t="s">
+        <v>268</v>
+      </c>
+      <c r="I16" t="s">
+        <v>173</v>
       </c>
       <c r="M16" t="s">
         <v>62</v>
@@ -1550,7 +1920,10 @@
         <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>18</v>
+      </c>
+      <c r="I17" t="s">
+        <v>174</v>
       </c>
       <c r="M17" t="s">
         <v>53</v>
@@ -1563,12 +1936,15 @@
       <c r="B18">
         <v>15</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="15"/>
       <c r="D18" t="s">
         <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="I18" t="s">
+        <v>175</v>
       </c>
       <c r="M18" t="s">
         <v>19</v>
@@ -1581,12 +1957,15 @@
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="15"/>
       <c r="D19" t="s">
         <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>155</v>
+      </c>
+      <c r="I19" t="s">
+        <v>176</v>
       </c>
       <c r="M19" t="s">
         <v>20</v>
@@ -1599,12 +1978,15 @@
       <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="15"/>
       <c r="D20" t="s">
         <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>156</v>
+      </c>
+      <c r="I20" t="s">
+        <v>177</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
@@ -1614,18 +1996,18 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>125</v>
-      </c>
       <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="15"/>
       <c r="D21" t="s">
         <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>157</v>
+      </c>
+      <c r="I21" t="s">
+        <v>178</v>
       </c>
       <c r="M21" t="s">
         <v>22</v>
@@ -1638,12 +2020,15 @@
       <c r="B22">
         <v>19</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="15"/>
       <c r="D22" t="s">
         <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>68</v>
+      </c>
+      <c r="I22" t="s">
+        <v>179</v>
       </c>
       <c r="M22" t="s">
         <v>23</v>
@@ -1656,12 +2041,15 @@
       <c r="B23">
         <v>20</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="15"/>
       <c r="D23" t="s">
         <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>158</v>
+      </c>
+      <c r="I23" t="s">
+        <v>180</v>
       </c>
       <c r="M23" t="s">
         <v>24</v>
@@ -1671,6 +2059,9 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
       <c r="B24">
         <v>21</v>
       </c>
@@ -1679,7 +2070,10 @@
         <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="I24" t="s">
+        <v>181</v>
       </c>
       <c r="M24" t="s">
         <v>25</v>
@@ -1697,7 +2091,13 @@
         <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>182</v>
+      </c>
+      <c r="H25" t="s">
+        <v>268</v>
+      </c>
+      <c r="I25" t="s">
+        <v>183</v>
       </c>
       <c r="M25" t="s">
         <v>26</v>
@@ -1717,6 +2117,9 @@
       <c r="E26" t="s">
         <v>24</v>
       </c>
+      <c r="I26" t="s">
+        <v>184</v>
+      </c>
       <c r="M26" t="s">
         <v>28</v>
       </c>
@@ -1735,6 +2138,12 @@
       <c r="E27" t="s">
         <v>54</v>
       </c>
+      <c r="G27" t="s">
+        <v>267</v>
+      </c>
+      <c r="I27" t="s">
+        <v>185</v>
+      </c>
       <c r="M27" t="s">
         <v>42</v>
       </c>
@@ -1743,15 +2152,24 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>129</v>
+      </c>
       <c r="B28">
         <v>25</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>209</v>
+      </c>
+      <c r="I28" t="s">
+        <v>186</v>
       </c>
       <c r="M28" t="s">
         <v>34</v>
@@ -1761,9 +2179,6 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>129</v>
-      </c>
       <c r="B29">
         <v>26</v>
       </c>
@@ -1772,7 +2187,10 @@
         <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>128</v>
+      </c>
+      <c r="I29" t="s">
+        <v>187</v>
       </c>
       <c r="M29" t="s">
         <v>29</v>
@@ -1782,15 +2200,24 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>130</v>
+      </c>
       <c r="B30">
         <v>27</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>28</v>
+      </c>
+      <c r="G30" t="s">
+        <v>208</v>
+      </c>
+      <c r="I30" t="s">
+        <v>188</v>
       </c>
       <c r="M30" t="s">
         <v>41</v>
@@ -1800,9 +2227,6 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>130</v>
-      </c>
       <c r="B31">
         <v>28</v>
       </c>
@@ -1811,7 +2235,10 @@
         <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>189</v>
+      </c>
+      <c r="I31" t="s">
+        <v>190</v>
       </c>
       <c r="M31" t="s">
         <v>30</v>
@@ -1829,7 +2256,10 @@
         <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>236</v>
+      </c>
+      <c r="I32" t="s">
+        <v>191</v>
       </c>
       <c r="M32" t="s">
         <v>35</v>
@@ -1849,6 +2279,9 @@
       <c r="E33" t="s">
         <v>34</v>
       </c>
+      <c r="I33" t="s">
+        <v>192</v>
+      </c>
       <c r="M33" t="s">
         <v>31</v>
       </c>
@@ -1870,6 +2303,12 @@
       <c r="E34" t="s">
         <v>29</v>
       </c>
+      <c r="G34" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34" t="s">
+        <v>197</v>
+      </c>
       <c r="M34" t="s">
         <v>40</v>
       </c>
@@ -1886,7 +2325,10 @@
         <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>41</v>
+        <v>196</v>
+      </c>
+      <c r="I35" t="s">
+        <v>195</v>
       </c>
       <c r="M35" t="s">
         <v>36</v>
@@ -1904,7 +2346,10 @@
         <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="I36" t="s">
+        <v>194</v>
       </c>
       <c r="M36" t="s">
         <v>32</v>
@@ -1922,7 +2367,10 @@
         <v>75</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="I37" t="s">
+        <v>193</v>
       </c>
       <c r="M37" t="s">
         <v>33</v>
@@ -1945,6 +2393,12 @@
       <c r="E38" t="s">
         <v>31</v>
       </c>
+      <c r="G38" t="s">
+        <v>206</v>
+      </c>
+      <c r="I38" t="s">
+        <v>198</v>
+      </c>
       <c r="M38" t="s">
         <v>37</v>
       </c>
@@ -1961,7 +2415,10 @@
         <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>154</v>
+      </c>
+      <c r="I39" t="s">
+        <v>199</v>
       </c>
       <c r="M39" t="s">
         <v>38</v>
@@ -1981,6 +2438,9 @@
       <c r="E40" t="s">
         <v>36</v>
       </c>
+      <c r="I40" t="s">
+        <v>200</v>
+      </c>
       <c r="M40" t="s">
         <v>39</v>
       </c>
@@ -2002,6 +2462,12 @@
       <c r="E41" t="s">
         <v>32</v>
       </c>
+      <c r="G41" t="s">
+        <v>205</v>
+      </c>
+      <c r="I41" t="s">
+        <v>201</v>
+      </c>
       <c r="M41" t="s">
         <v>43</v>
       </c>
@@ -2018,7 +2484,10 @@
         <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>204</v>
+      </c>
+      <c r="I42" t="s">
+        <v>203</v>
       </c>
       <c r="M42" t="s">
         <v>44</v>
@@ -2038,6 +2507,9 @@
       <c r="E43" t="s">
         <v>37</v>
       </c>
+      <c r="I43" t="s">
+        <v>202</v>
+      </c>
       <c r="M43" t="s">
         <v>47</v>
       </c>
@@ -2059,6 +2531,12 @@
       <c r="E44" t="s">
         <v>38</v>
       </c>
+      <c r="G44" t="s">
+        <v>210</v>
+      </c>
+      <c r="I44" t="s">
+        <v>211</v>
+      </c>
       <c r="M44" t="s">
         <v>45</v>
       </c>
@@ -2077,6 +2555,9 @@
       <c r="E45" t="s">
         <v>39</v>
       </c>
+      <c r="I45" t="s">
+        <v>212</v>
+      </c>
       <c r="M45" t="s">
         <v>46</v>
       </c>
@@ -2095,6 +2576,9 @@
       <c r="E46" t="s">
         <v>43</v>
       </c>
+      <c r="I46" t="s">
+        <v>213</v>
+      </c>
       <c r="M46" t="s">
         <v>48</v>
       </c>
@@ -2116,6 +2600,12 @@
       <c r="E47" t="s">
         <v>44</v>
       </c>
+      <c r="G47" t="s">
+        <v>224</v>
+      </c>
+      <c r="I47" t="s">
+        <v>217</v>
+      </c>
       <c r="M47" t="s">
         <v>49</v>
       </c>
@@ -2134,6 +2624,9 @@
       <c r="E48" t="s">
         <v>47</v>
       </c>
+      <c r="I48" t="s">
+        <v>223</v>
+      </c>
       <c r="M48" t="s">
         <v>50</v>
       </c>
@@ -2150,7 +2643,10 @@
         <v>78</v>
       </c>
       <c r="E49" t="s">
-        <v>45</v>
+        <v>214</v>
+      </c>
+      <c r="I49" t="s">
+        <v>222</v>
       </c>
       <c r="M49" t="s">
         <v>56</v>
@@ -2168,7 +2664,10 @@
         <v>78</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
+        <v>215</v>
+      </c>
+      <c r="I50" t="s">
+        <v>221</v>
       </c>
       <c r="M50" t="s">
         <v>51</v>
@@ -2186,10 +2685,13 @@
       </c>
       <c r="C51" s="10"/>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E51" t="s">
-        <v>48</v>
+        <v>216</v>
+      </c>
+      <c r="I51" t="s">
+        <v>220</v>
       </c>
       <c r="M51" t="s">
         <v>128</v>
@@ -2204,10 +2706,13 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E52" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="I52" t="s">
+        <v>219</v>
       </c>
       <c r="M52" t="s">
         <v>52</v>
@@ -2222,10 +2727,13 @@
       </c>
       <c r="C53" s="10"/>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E53" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="I53" t="s">
+        <v>218</v>
       </c>
       <c r="M53" t="s">
         <v>54</v>
@@ -2235,18 +2743,24 @@
       </c>
     </row>
     <row r="54" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
-        <v>138</v>
+      <c r="A54" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="B54">
         <v>51</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="G54" t="s">
+        <v>231</v>
+      </c>
+      <c r="I54" t="s">
+        <v>227</v>
       </c>
       <c r="M54" t="s">
         <v>55</v>
@@ -2256,15 +2770,19 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="13"/>
       <c r="B55">
         <v>52</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E55" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="I55" t="s">
+        <v>226</v>
       </c>
       <c r="M55" t="s">
         <v>66</v>
@@ -2274,18 +2792,18 @@
       </c>
     </row>
     <row r="56" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>142</v>
-      </c>
       <c r="B56">
         <v>53</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E56" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="I56" t="s">
+        <v>225</v>
       </c>
       <c r="M56" t="s">
         <v>67</v>
@@ -2295,15 +2813,24 @@
       </c>
     </row>
     <row r="57" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>261</v>
+      </c>
       <c r="B57">
         <v>54</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="E57" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="G57" t="s">
+        <v>235</v>
+      </c>
+      <c r="I57" t="s">
+        <v>228</v>
       </c>
       <c r="M57" t="s">
         <v>68</v>
@@ -2313,21 +2840,18 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>139</v>
-      </c>
       <c r="B58">
         <v>55</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="E58" t="s">
-        <v>158</v>
+        <v>51</v>
       </c>
       <c r="I58" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="M58" t="s">
         <v>69</v>
@@ -2340,15 +2864,18 @@
       <c r="B59">
         <v>56</v>
       </c>
-      <c r="C59" s="10"/>
+      <c r="C59" s="15"/>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>52</v>
+      </c>
+      <c r="G59" t="s">
+        <v>234</v>
       </c>
       <c r="I59" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
       <c r="M59" t="s">
         <v>70</v>
@@ -2361,15 +2888,15 @@
       <c r="B60">
         <v>57</v>
       </c>
-      <c r="C60" s="10"/>
+      <c r="C60" s="15"/>
       <c r="D60" t="s">
-        <v>162</v>
+        <v>262</v>
       </c>
       <c r="E60" t="s">
-        <v>149</v>
+        <v>263</v>
       </c>
       <c r="I60" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="M60" t="s">
         <v>71</v>
@@ -2379,18 +2906,21 @@
       </c>
     </row>
     <row r="61" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>138</v>
+      </c>
       <c r="B61">
         <v>58</v>
       </c>
-      <c r="C61" s="10"/>
+      <c r="C61" s="15"/>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>246</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>247</v>
       </c>
       <c r="I61" t="s">
-        <v>160</v>
+        <v>248</v>
       </c>
       <c r="M61" t="s">
         <v>72</v>
@@ -2403,39 +2933,42 @@
       <c r="B62">
         <v>59</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="15"/>
       <c r="D62" t="s">
-        <v>155</v>
+        <v>266</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>249</v>
+      </c>
+      <c r="G62" t="s">
+        <v>237</v>
       </c>
       <c r="I62" t="s">
-        <v>161</v>
+        <v>257</v>
       </c>
       <c r="M62" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>141</v>
-      </c>
       <c r="B63">
         <v>60</v>
       </c>
-      <c r="C63" s="15"/>
+      <c r="C63" s="10"/>
       <c r="D63" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>141</v>
+      </c>
+      <c r="G63" t="s">
+        <v>250</v>
       </c>
       <c r="I63" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M63" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2444,16 +2977,19 @@
       </c>
       <c r="C64" s="15"/>
       <c r="D64" t="s">
-        <v>80</v>
+        <v>238</v>
       </c>
       <c r="E64" t="s">
-        <v>71</v>
+        <v>242</v>
+      </c>
+      <c r="G64" t="s">
+        <v>251</v>
       </c>
       <c r="I64" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="M64" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2462,31 +2998,37 @@
       </c>
       <c r="C65" s="15"/>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>252</v>
       </c>
       <c r="E65" t="s">
-        <v>72</v>
+        <v>253</v>
+      </c>
+      <c r="G65" t="s">
+        <v>255</v>
       </c>
       <c r="I65" t="s">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="M65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>146</v>
-      </c>
       <c r="B66">
         <v>63</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" s="15"/>
       <c r="D66" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
       <c r="E66" t="s">
-        <v>63</v>
+        <v>240</v>
+      </c>
+      <c r="G66" t="s">
+        <v>254</v>
+      </c>
+      <c r="I66" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2495,10 +3037,115 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" t="s">
+        <v>256</v>
+      </c>
+      <c r="E67" t="s">
+        <v>145</v>
+      </c>
+      <c r="G67" t="s">
+        <v>265</v>
+      </c>
+      <c r="I67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68">
+        <v>65</v>
+      </c>
+      <c r="C68" s="15"/>
+      <c r="D68" t="s">
+        <v>245</v>
+      </c>
+      <c r="E68" t="s">
+        <v>244</v>
+      </c>
+      <c r="G68" t="s">
+        <v>150</v>
+      </c>
+      <c r="I68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B69">
+        <v>66</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" t="s">
+        <v>70</v>
+      </c>
+      <c r="I69" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70">
+        <v>67</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="I70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+      <c r="I71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72">
+        <v>69</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" t="s">
+        <v>63</v>
+      </c>
+      <c r="I72" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73">
+        <v>70</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" t="s">
         <v>127</v>
       </c>
-      <c r="E67" t="s">
-        <v>62</v>
+      <c r="E73" t="s">
+        <v>260</v>
+      </c>
+      <c r="I73" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wwise Audio Asset Calibrations
</commit_message>
<xml_diff>
--- a/Assets/Audio/Silent Space Audio Asset List.xlsx
+++ b/Assets/Audio/Silent Space Audio Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/Assets/Audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34CBE6A-6D0F-5A4A-8A66-AABBA3BF16CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A23B3-5152-2C4A-9D2F-10BB7BD25BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52620" yWindow="7700" windowWidth="36980" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1523,8 +1523,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Documentation and Wwise Calibration Update
</commit_message>
<xml_diff>
--- a/Assets/Audio/Silent Space Audio Asset List.xlsx
+++ b/Assets/Audio/Silent Space Audio Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/Assets/Audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A23B3-5152-2C4A-9D2F-10BB7BD25BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8514FDA6-AD28-0740-B4D8-DB9A31A7F9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52620" yWindow="7700" windowWidth="36980" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57400" yWindow="7700" windowWidth="32120" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SFX" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="269">
   <si>
     <t>Sound Effect Asset List</t>
   </si>
@@ -83,9 +83,6 @@
     <t>WMII - Silent Space</t>
   </si>
   <si>
-    <t>SFX NAME</t>
-  </si>
-  <si>
     <t>Stun Gun Fire</t>
   </si>
   <si>
@@ -846,6 +843,9 @@
   </si>
   <si>
     <t>Step Playlist Container</t>
+  </si>
+  <si>
+    <t>Event Name</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,6 +972,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1011,7 +1017,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1062,6 +1068,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="5" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="5" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1200,10 +1212,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959B0350-8070-1649-9BA9-4FE5A44B2E5C}" name="Table172" displayName="Table172" ref="M3:N65" totalsRowShown="0">
-  <autoFilter ref="M3:N65" xr:uid="{959B0350-8070-1649-9BA9-4FE5A44B2E5C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959B0350-8070-1649-9BA9-4FE5A44B2E5C}" name="Table172" displayName="Table172" ref="M3:N73" totalsRowShown="0">
+  <autoFilter ref="M3:N73" xr:uid="{959B0350-8070-1649-9BA9-4FE5A44B2E5C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5AE1BA70-ED06-5449-93AF-26CED737BC02}" name="SFX NAME"/>
+    <tableColumn id="1" xr3:uid="{5AE1BA70-ED06-5449-93AF-26CED737BC02}" name="Event Name"/>
     <tableColumn id="2" xr3:uid="{28BDB086-EE9F-4040-BF55-4606B3DADDE9}" name="gameObject"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1523,8 +1535,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C71" sqref="C69:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1556,7 +1568,7 @@
     </row>
     <row r="3" spans="1:14" ht="22.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1589,119 +1601,119 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="17"/>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="17"/>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="17"/>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="17"/>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" t="s">
+        <v>267</v>
+      </c>
+      <c r="I7" t="s">
         <v>168</v>
-      </c>
-      <c r="H7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I7" t="s">
-        <v>169</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" t="s">
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1710,181 +1722,181 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M8" t="s">
         <v>64</v>
       </c>
-      <c r="I8" t="s">
-        <v>162</v>
-      </c>
-      <c r="M8" t="s">
-        <v>65</v>
-      </c>
       <c r="N8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="17"/>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="17"/>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="17"/>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K11" s="11"/>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="17"/>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K12" s="11"/>
       <c r="M12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="17"/>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K13" s="11"/>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14">
         <v>11</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="17"/>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>170</v>
+      </c>
+      <c r="M14" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
-        <v>171</v>
-      </c>
-      <c r="M14" t="s">
-        <v>18</v>
-      </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15">
         <v>12</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="17"/>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1893,22 +1905,22 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -1917,169 +1929,169 @@
       </c>
       <c r="C17" s="10"/>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18">
         <v>15</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="18"/>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="18"/>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="18"/>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="18"/>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22">
         <v>19</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="17"/>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23">
         <v>20</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="17"/>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24">
         <v>21</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2088,22 +2100,22 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" t="s">
+        <v>267</v>
+      </c>
+      <c r="I25" t="s">
         <v>182</v>
       </c>
-      <c r="H25" t="s">
-        <v>268</v>
-      </c>
-      <c r="I25" t="s">
-        <v>183</v>
-      </c>
       <c r="M25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2112,19 +2124,19 @@
       </c>
       <c r="C26" s="10"/>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2133,49 +2145,49 @@
       </c>
       <c r="C27" s="10"/>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28">
         <v>25</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2184,136 +2196,136 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30">
         <v>27</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="15"/>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31">
         <v>28</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="15"/>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
+        <v>188</v>
+      </c>
+      <c r="I31" t="s">
         <v>189</v>
       </c>
-      <c r="I31" t="s">
-        <v>190</v>
-      </c>
       <c r="M31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>29</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="15"/>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33">
         <v>30</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="15"/>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B34">
         <v>31</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I34" t="s">
+        <v>196</v>
+      </c>
+      <c r="M34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" t="s">
         <v>75</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" t="s">
-        <v>207</v>
-      </c>
-      <c r="I34" t="s">
-        <v>197</v>
-      </c>
-      <c r="M34" t="s">
-        <v>40</v>
-      </c>
-      <c r="N34" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2322,19 +2334,19 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
+        <v>195</v>
+      </c>
+      <c r="I35" t="s">
+        <v>194</v>
+      </c>
+      <c r="M35" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35" t="s">
         <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>196</v>
-      </c>
-      <c r="I35" t="s">
-        <v>195</v>
-      </c>
-      <c r="M35" t="s">
-        <v>36</v>
-      </c>
-      <c r="N35" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2343,19 +2355,19 @@
       </c>
       <c r="C36" s="10"/>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2364,46 +2376,46 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38">
         <v>35</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>205</v>
+      </c>
+      <c r="I38" t="s">
+        <v>197</v>
+      </c>
+      <c r="M38" t="s">
+        <v>36</v>
+      </c>
+      <c r="N38" t="s">
         <v>76</v>
-      </c>
-      <c r="E38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" t="s">
-        <v>206</v>
-      </c>
-      <c r="I38" t="s">
-        <v>198</v>
-      </c>
-      <c r="M38" t="s">
-        <v>37</v>
-      </c>
-      <c r="N38" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2412,19 +2424,19 @@
       </c>
       <c r="C39" s="10"/>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2433,46 +2445,46 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41">
         <v>38</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2481,19 +2493,19 @@
       </c>
       <c r="C42" s="10"/>
       <c r="D42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" t="s">
+        <v>203</v>
+      </c>
+      <c r="I42" t="s">
+        <v>202</v>
+      </c>
+      <c r="M42" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" t="s">
         <v>77</v>
-      </c>
-      <c r="E42" t="s">
-        <v>204</v>
-      </c>
-      <c r="I42" t="s">
-        <v>203</v>
-      </c>
-      <c r="M42" t="s">
-        <v>44</v>
-      </c>
-      <c r="N42" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2502,46 +2514,46 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>201</v>
+      </c>
+      <c r="M43" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43" t="s">
         <v>77</v>
-      </c>
-      <c r="E43" t="s">
-        <v>37</v>
-      </c>
-      <c r="I43" t="s">
-        <v>202</v>
-      </c>
-      <c r="M43" t="s">
-        <v>47</v>
-      </c>
-      <c r="N43" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44">
         <v>41</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G44" t="s">
+        <v>209</v>
+      </c>
+      <c r="I44" t="s">
         <v>210</v>
       </c>
-      <c r="I44" t="s">
-        <v>211</v>
-      </c>
       <c r="M44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2550,19 +2562,19 @@
       </c>
       <c r="C45" s="10"/>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2571,46 +2583,46 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" t="s">
+        <v>212</v>
+      </c>
+      <c r="M46" t="s">
+        <v>47</v>
+      </c>
+      <c r="N46" t="s">
         <v>82</v>
-      </c>
-      <c r="E46" t="s">
-        <v>43</v>
-      </c>
-      <c r="I46" t="s">
-        <v>213</v>
-      </c>
-      <c r="M46" t="s">
-        <v>48</v>
-      </c>
-      <c r="N46" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B47">
         <v>44</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2619,19 +2631,19 @@
       </c>
       <c r="C48" s="10"/>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2640,19 +2652,19 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" t="s">
+        <v>213</v>
+      </c>
+      <c r="I49" t="s">
+        <v>221</v>
+      </c>
+      <c r="M49" t="s">
+        <v>55</v>
+      </c>
+      <c r="N49" t="s">
         <v>78</v>
-      </c>
-      <c r="E49" t="s">
-        <v>214</v>
-      </c>
-      <c r="I49" t="s">
-        <v>222</v>
-      </c>
-      <c r="M49" t="s">
-        <v>56</v>
-      </c>
-      <c r="N49" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2661,43 +2673,43 @@
       </c>
       <c r="C50" s="10"/>
       <c r="D50" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" t="s">
+        <v>214</v>
+      </c>
+      <c r="I50" t="s">
+        <v>220</v>
+      </c>
+      <c r="M50" t="s">
+        <v>50</v>
+      </c>
+      <c r="N50" t="s">
         <v>78</v>
-      </c>
-      <c r="E50" t="s">
-        <v>215</v>
-      </c>
-      <c r="I50" t="s">
-        <v>221</v>
-      </c>
-      <c r="M50" t="s">
-        <v>51</v>
-      </c>
-      <c r="N50" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51">
         <v>48</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2706,19 +2718,19 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2727,46 +2739,46 @@
       </c>
       <c r="C53" s="10"/>
       <c r="D53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B54">
         <v>51</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2776,19 +2788,19 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2797,46 +2809,46 @@
       </c>
       <c r="C56" s="10"/>
       <c r="D56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B57">
         <v>54</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G57" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2845,109 +2857,112 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59">
         <v>56</v>
       </c>
-      <c r="C59" s="15"/>
+      <c r="C59" s="17"/>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60">
         <v>57</v>
       </c>
-      <c r="C60" s="15"/>
+      <c r="C60" s="17"/>
       <c r="D60" t="s">
+        <v>261</v>
+      </c>
+      <c r="E60" t="s">
         <v>262</v>
       </c>
-      <c r="E60" t="s">
+      <c r="I60" t="s">
         <v>263</v>
       </c>
-      <c r="I60" t="s">
-        <v>264</v>
-      </c>
       <c r="M60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B61">
         <v>58</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" s="17"/>
       <c r="D61" t="s">
+        <v>245</v>
+      </c>
+      <c r="E61" t="s">
         <v>246</v>
       </c>
-      <c r="E61" t="s">
+      <c r="I61" t="s">
         <v>247</v>
       </c>
-      <c r="I61" t="s">
-        <v>248</v>
-      </c>
       <c r="M61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62">
         <v>59</v>
       </c>
-      <c r="C62" s="15"/>
+      <c r="C62" s="17"/>
       <c r="D62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M62" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="N62" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -2956,196 +2971,205 @@
       </c>
       <c r="C63" s="10"/>
       <c r="D63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M63" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="N63" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64">
         <v>61</v>
       </c>
-      <c r="C64" s="15"/>
+      <c r="C64" s="17"/>
       <c r="D64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E64" t="s">
+        <v>241</v>
+      </c>
+      <c r="G64" t="s">
+        <v>250</v>
+      </c>
+      <c r="I64" t="s">
         <v>242</v>
       </c>
-      <c r="G64" t="s">
-        <v>251</v>
-      </c>
-      <c r="I64" t="s">
-        <v>243</v>
-      </c>
       <c r="M64" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+      <c r="N64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B65">
         <v>62</v>
       </c>
-      <c r="C65" s="15"/>
+      <c r="C65" s="17"/>
       <c r="D65" t="s">
+        <v>251</v>
+      </c>
+      <c r="E65" t="s">
         <v>252</v>
       </c>
-      <c r="E65" t="s">
-        <v>253</v>
-      </c>
       <c r="G65" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I65" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M65" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+      <c r="N65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66">
         <v>63</v>
       </c>
-      <c r="C66" s="15"/>
+      <c r="C66" s="17"/>
       <c r="D66" t="s">
+        <v>238</v>
+      </c>
+      <c r="E66" t="s">
         <v>239</v>
       </c>
-      <c r="E66" t="s">
+      <c r="G66" t="s">
+        <v>253</v>
+      </c>
+      <c r="I66" t="s">
         <v>240</v>
       </c>
-      <c r="G66" t="s">
-        <v>254</v>
-      </c>
-      <c r="I66" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="67" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B67">
         <v>64</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I67" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68">
         <v>65</v>
       </c>
-      <c r="C68" s="15"/>
+      <c r="C68" s="17"/>
       <c r="D68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E68" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I68" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B69">
         <v>66</v>
       </c>
-      <c r="C69" s="15"/>
+      <c r="C69" s="17"/>
       <c r="D69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I69" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B70">
         <v>67</v>
       </c>
-      <c r="C70" s="15"/>
+      <c r="C70" s="17"/>
       <c r="D70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I70" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B71">
         <v>68</v>
       </c>
-      <c r="C71" s="15"/>
+      <c r="C71" s="17"/>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I71" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B72">
         <v>69</v>
       </c>
-      <c r="C72" s="15"/>
+      <c r="C72" s="17"/>
       <c r="D72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I72" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B73">
         <v>70</v>
       </c>
-      <c r="C73" s="15"/>
+      <c r="C73" s="18"/>
       <c r="D73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E73" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3198,7 +3222,7 @@
     </row>
     <row r="2" spans="1:13" ht="24" x14ac:dyDescent="0.15">
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3222,7 +3246,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
@@ -3234,25 +3258,25 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" t="s">
@@ -3260,25 +3284,25 @@
       </c>
       <c r="K4" s="12"/>
       <c r="L4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
-        <v>109</v>
-      </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" t="s">
@@ -3286,25 +3310,25 @@
       </c>
       <c r="K5" s="12"/>
       <c r="L5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="10"/>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" t="s">
@@ -3312,208 +3336,208 @@
       </c>
       <c r="K6" s="12"/>
       <c r="L6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
         <v>88</v>
       </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="10"/>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="10"/>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="10"/>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="10"/>
       <c r="C17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="10"/>
       <c r="C18" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="10"/>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" t="s">
         <v>113</v>
-      </c>
-      <c r="F19" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Enemy Ambiences and Area Ambiences Correctly
</commit_message>
<xml_diff>
--- a/Assets/Audio/Silent Space Audio Asset List.xlsx
+++ b/Assets/Audio/Silent Space Audio Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/Assets/Audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B327A2-667E-7941-ABBA-F1E96FB55558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E4E862-C58F-CB41-8114-C904B20269B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57400" yWindow="7700" windowWidth="32120" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="241">
   <si>
     <t>Sound Effect Asset List</t>
   </si>
@@ -485,15 +485,9 @@
     <t>sfx_ui_pause.wav</t>
   </si>
   <si>
-    <t>Safe Room</t>
-  </si>
-  <si>
     <t>Boss Room</t>
   </si>
   <si>
-    <t>sfx_ambience_safe</t>
-  </si>
-  <si>
     <t>sfx_ambience_boss</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>sfx_player_stun_cooldown</t>
   </si>
   <si>
-    <t>sfx_player_emp</t>
-  </si>
-  <si>
     <t>sfx_player_grenade_fire</t>
   </si>
   <si>
@@ -560,9 +551,6 @@
     <t>sfx_player_jetpack_fuel_meter</t>
   </si>
   <si>
-    <t>sfx_player_jetpack_fuel_ultimate</t>
-  </si>
-  <si>
     <t>sfx_player_footsteps_metal_#</t>
   </si>
   <si>
@@ -590,18 +578,9 @@
     <t>sfx_noise_meter_trigger_#</t>
   </si>
   <si>
-    <t>sfx_noise_meter_tentacle_element</t>
-  </si>
-  <si>
     <t>sfx_player_instant_kill</t>
   </si>
   <si>
-    <t>sfx_enemie_tentacle_spawn</t>
-  </si>
-  <si>
-    <t>sfx_enemie_tentacle_ambience</t>
-  </si>
-  <si>
     <t>sfx_enemie_infected_idle</t>
   </si>
   <si>
@@ -611,24 +590,12 @@
     <t>sfx_enemie_infected_hurt_#</t>
   </si>
   <si>
-    <t>sfx_enemie_infected_attacking_#</t>
-  </si>
-  <si>
     <t>sfx_enemie_infected_death_#</t>
   </si>
   <si>
     <t>sfx_enemie_crawlers_explode</t>
   </si>
   <si>
-    <t>sfx_enemie_crawlers_attacking</t>
-  </si>
-  <si>
-    <t>sfx_enemie_crawlers_hurt</t>
-  </si>
-  <si>
-    <t>Crawlers Hurt</t>
-  </si>
-  <si>
     <t>sfx_enemie_crawlers_idle</t>
   </si>
   <si>
@@ -644,15 +611,6 @@
     <t>sfx_enemie_glob_idle</t>
   </si>
   <si>
-    <t>sfx_enemie_glob_death</t>
-  </si>
-  <si>
-    <t>sfx_enemie_glob_attacking</t>
-  </si>
-  <si>
-    <t>Glob Alerted?</t>
-  </si>
-  <si>
     <t>jellyfish like creatures</t>
   </si>
   <si>
@@ -665,9 +623,6 @@
     <t>infected crew members</t>
   </si>
   <si>
-    <t>tentacles</t>
-  </si>
-  <si>
     <t>giant overgrown infected blob</t>
   </si>
   <si>
@@ -686,9 +641,6 @@
     <t>Xeno-encephalon Gas Attack</t>
   </si>
   <si>
-    <t>Xeno-encephalon Head Slam</t>
-  </si>
-  <si>
     <t>sfx_enemie_xeno-encephalon_idle</t>
   </si>
   <si>
@@ -698,42 +650,15 @@
     <t>sfx_enemie_xeno-encephalon_damaged</t>
   </si>
   <si>
-    <t>sfx_enemie_xeno-encephalon_head_slam</t>
-  </si>
-  <si>
     <t>sfx_enemie_xeno-encephalon_gas_attack</t>
   </si>
   <si>
     <t>sfx_enemie_xeno-encephalon_attack_through_surface</t>
   </si>
   <si>
-    <t>sfx_enemie_xeno-encephalon_movement</t>
-  </si>
-  <si>
-    <t>boss of the game - two skeleton heads with a brain for a body</t>
-  </si>
-  <si>
-    <t>sfx_enemie_eye_stalker_death</t>
-  </si>
-  <si>
-    <t>sfx_enemie_eye_stalker_alerted</t>
-  </si>
-  <si>
-    <t>sfx_enemie_eye_stalker_idle</t>
-  </si>
-  <si>
-    <t>sfx_environment_fungus_destoryed</t>
-  </si>
-  <si>
-    <t>sfx_environment_fungus_ambience</t>
-  </si>
-  <si>
     <t>sfx_environment_security_alarm_activated</t>
   </si>
   <si>
-    <t>small eye of xeno-encephalon that follows the player and increases the noise meter</t>
-  </si>
-  <si>
     <t>sfx_objects_alien_artifact_#</t>
   </si>
   <si>
@@ -743,12 +668,6 @@
     <t>increases noise meter</t>
   </si>
   <si>
-    <t>blocks player's path</t>
-  </si>
-  <si>
-    <t>Infected Attacking</t>
-  </si>
-  <si>
     <t>0 Gravity Room</t>
   </si>
   <si>
@@ -788,9 +707,6 @@
     <t>Ship Hull Ambience</t>
   </si>
   <si>
-    <t>Room that holds constellation keys</t>
-  </si>
-  <si>
     <t>Alien monologues are used in this area</t>
   </si>
   <si>
@@ -806,18 +722,12 @@
     <t>where the infected alien artifact was found</t>
   </si>
   <si>
-    <t>General Areas</t>
-  </si>
-  <si>
     <t>sfx_ambience_ship_hull</t>
   </si>
   <si>
     <t>sfx_ambience_warehouse</t>
   </si>
   <si>
-    <t>sfx_ambience_general</t>
-  </si>
-  <si>
     <t>Voice Log Activation (6)</t>
   </si>
   <si>
@@ -833,9 +743,6 @@
     <t>sfx_environment_elevator</t>
   </si>
   <si>
-    <t>A general track for ambience in other non key areas</t>
-  </si>
-  <si>
     <t>Ship Hull</t>
   </si>
   <si>
@@ -846,6 +753,15 @@
   </si>
   <si>
     <t>Event Name</t>
+  </si>
+  <si>
+    <t>Health Bar Replenish Pick-Up</t>
+  </si>
+  <si>
+    <t>Jetpack Fuel Pick-Up</t>
+  </si>
+  <si>
+    <t>boss of the game - brain ambiance</t>
   </si>
 </sst>
 </file>
@@ -962,12 +878,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -981,6 +891,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,17 +985,17 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="5" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="5" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="5" applyFill="1">
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="0" xfId="5" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1188,8 +1104,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="C3:J73" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="C3:J73" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="C3:J54" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="C3:J54" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="STATUS" dataDxfId="3" dataCellStyle="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="LOCATION"/>
@@ -1544,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:J53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1610,7 +1526,7 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="N3" t="s">
         <v>26</v>
@@ -1631,11 +1547,11 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" s="16"/>
+        <v>156</v>
+      </c>
+      <c r="K4" s="15"/>
       <c r="L4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -1649,18 +1565,21 @@
         <v>2</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H5" t="s">
-        <v>267</v>
-      </c>
-      <c r="I5" t="s">
-        <v>159</v>
-      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" s="19"/>
       <c r="K5" s="7"/>
       <c r="L5" t="s">
         <v>3</v>
@@ -1677,15 +1596,19 @@
         <v>3</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I6" t="s">
-        <v>160</v>
-      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="19"/>
       <c r="K6" s="8"/>
       <c r="L6" t="s">
         <v>4</v>
@@ -1702,18 +1625,21 @@
         <v>4</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>167</v>
-      </c>
-      <c r="H7" t="s">
-        <v>267</v>
-      </c>
-      <c r="I7" t="s">
-        <v>168</v>
-      </c>
+      <c r="D7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" s="19"/>
       <c r="K7" s="9"/>
       <c r="L7" t="s">
         <v>5</v>
@@ -1729,16 +1655,20 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" t="s">
-        <v>161</v>
-      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="18"/>
       <c r="M8" t="s">
         <v>64</v>
       </c>
@@ -1755,10 +1685,10 @@
         <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="I9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M9" t="s">
         <v>59</v>
@@ -1776,10 +1706,13 @@
         <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>236</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M10" t="s">
         <v>58</v>
@@ -1792,19 +1725,20 @@
       <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" t="s">
-        <v>267</v>
-      </c>
-      <c r="I11" t="s">
-        <v>164</v>
-      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J11" s="18"/>
       <c r="K11" s="11"/>
       <c r="M11" t="s">
         <v>16</v>
@@ -1817,16 +1751,22 @@
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="I12" t="s">
-        <v>165</v>
-      </c>
+      <c r="J12" s="18"/>
       <c r="K12" s="11"/>
       <c r="M12" t="s">
         <v>57</v>
@@ -1847,13 +1787,10 @@
         <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>267</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K13" s="11"/>
       <c r="M13" t="s">
@@ -1872,10 +1809,13 @@
         <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>236</v>
       </c>
       <c r="I14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M14" t="s">
         <v>17</v>
@@ -1889,18 +1829,21 @@
         <v>12</v>
       </c>
       <c r="C15" s="17"/>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" t="s">
-        <v>267</v>
-      </c>
-      <c r="I15" t="s">
-        <v>171</v>
-      </c>
+      <c r="D15" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="19"/>
       <c r="M15" t="s">
         <v>62</v>
       </c>
@@ -1912,18 +1855,15 @@
       <c r="B16">
         <v>13</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="17"/>
       <c r="D16" t="s">
         <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" t="s">
-        <v>267</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M16" t="s">
         <v>61</v>
@@ -1936,15 +1876,15 @@
       <c r="B17">
         <v>14</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="17"/>
       <c r="D17" t="s">
         <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="I17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M17" t="s">
         <v>52</v>
@@ -1957,15 +1897,15 @@
       <c r="B18">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="17"/>
       <c r="D18" t="s">
         <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="I18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
@@ -1978,7 +1918,7 @@
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="17"/>
       <c r="D19" t="s">
         <v>73</v>
       </c>
@@ -1986,7 +1926,7 @@
         <v>154</v>
       </c>
       <c r="I19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M19" t="s">
         <v>19</v>
@@ -1999,15 +1939,15 @@
       <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="17"/>
       <c r="D20" t="s">
         <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
@@ -2020,15 +1960,15 @@
       <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="17"/>
       <c r="D21" t="s">
         <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M21" t="s">
         <v>21</v>
@@ -2042,15 +1982,19 @@
         <v>19</v>
       </c>
       <c r="C22" s="17"/>
-      <c r="D22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>178</v>
-      </c>
+      <c r="D22" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="J22" s="19"/>
       <c r="M22" t="s">
         <v>22</v>
       </c>
@@ -2062,16 +2006,22 @@
       <c r="B23">
         <v>20</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" t="s">
-        <v>179</v>
-      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J23" s="18"/>
       <c r="M23" t="s">
         <v>23</v>
       </c>
@@ -2086,16 +2036,22 @@
       <c r="B24">
         <v>21</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" t="s">
-        <v>180</v>
-      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="J24" s="19"/>
       <c r="M24" t="s">
         <v>24</v>
       </c>
@@ -2107,18 +2063,18 @@
       <c r="B25">
         <v>22</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="17"/>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H25" t="s">
-        <v>267</v>
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>193</v>
       </c>
       <c r="I25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M25" t="s">
         <v>25</v>
@@ -2131,15 +2087,15 @@
       <c r="B26">
         <v>23</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="17"/>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="I26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M26" t="s">
         <v>27</v>
@@ -2152,18 +2108,15 @@
       <c r="B27">
         <v>24</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="17"/>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" t="s">
-        <v>266</v>
+        <v>33</v>
       </c>
       <c r="I27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M27" t="s">
         <v>41</v>
@@ -2179,19 +2132,22 @@
       <c r="B28">
         <v>25</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
-        <v>208</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19" t="s">
         <v>185</v>
       </c>
+      <c r="J28" s="19"/>
       <c r="M28" t="s">
         <v>33</v>
       </c>
@@ -2203,16 +2159,20 @@
       <c r="B29">
         <v>26</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
-        <v>127</v>
-      </c>
-      <c r="I29" t="s">
-        <v>186</v>
-      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="J29" s="19"/>
       <c r="M29" t="s">
         <v>28</v>
       </c>
@@ -2227,18 +2187,18 @@
       <c r="B30">
         <v>27</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="17"/>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M30" t="s">
         <v>40</v>
@@ -2251,15 +2211,15 @@
       <c r="B31">
         <v>28</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="17"/>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E31" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="I31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M31" t="s">
         <v>29</v>
@@ -2272,15 +2232,15 @@
       <c r="B32">
         <v>29</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="17"/>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>235</v>
+        <v>35</v>
       </c>
       <c r="I32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M32" t="s">
         <v>34</v>
@@ -2293,16 +2253,22 @@
       <c r="B33">
         <v>30</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" t="s">
-        <v>191</v>
-      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" s="19"/>
       <c r="M33" t="s">
         <v>30</v>
       </c>
@@ -2317,19 +2283,22 @@
       <c r="B34">
         <v>31</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" t="s">
-        <v>206</v>
-      </c>
-      <c r="I34" t="s">
-        <v>196</v>
-      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="J34" s="19"/>
       <c r="M34" t="s">
         <v>39</v>
       </c>
@@ -2341,18 +2310,18 @@
       <c r="B35">
         <v>32</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="19" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>195</v>
+        <v>38</v>
       </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J35" s="19"/>
       <c r="M35" t="s">
@@ -2366,18 +2335,18 @@
       <c r="B36">
         <v>33</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="19" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="J36" s="19"/>
       <c r="M36" t="s">
@@ -2391,16 +2360,22 @@
       <c r="B37">
         <v>34</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" t="s">
-        <v>192</v>
-      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="J37" s="19"/>
       <c r="M37" t="s">
         <v>32</v>
       </c>
@@ -2415,19 +2390,20 @@
       <c r="B38">
         <v>35</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" t="s">
-        <v>30</v>
-      </c>
-      <c r="G38" t="s">
-        <v>205</v>
-      </c>
-      <c r="I38" t="s">
-        <v>197</v>
-      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J38" s="19"/>
       <c r="M38" t="s">
         <v>36</v>
       </c>
@@ -2439,16 +2415,20 @@
       <c r="B39">
         <v>36</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" t="s">
-        <v>153</v>
-      </c>
-      <c r="I39" t="s">
-        <v>198</v>
-      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="J39" s="19"/>
       <c r="M39" t="s">
         <v>37</v>
       </c>
@@ -2460,16 +2440,20 @@
       <c r="B40">
         <v>37</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" t="s">
-        <v>35</v>
-      </c>
-      <c r="I40" t="s">
-        <v>199</v>
-      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="J40" s="19"/>
       <c r="M40" t="s">
         <v>38</v>
       </c>
@@ -2484,19 +2468,20 @@
       <c r="B41">
         <v>38</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" t="s">
-        <v>204</v>
-      </c>
-      <c r="I41" t="s">
-        <v>200</v>
-      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="19"/>
       <c r="M41" t="s">
         <v>42</v>
       </c>
@@ -2508,20 +2493,19 @@
       <c r="B42">
         <v>39</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="J42" s="19"/>
+      <c r="C42" s="16"/>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" t="s">
+        <v>208</v>
+      </c>
+      <c r="I42" t="s">
+        <v>205</v>
+      </c>
       <c r="M42" t="s">
         <v>43</v>
       </c>
@@ -2533,20 +2517,16 @@
       <c r="B43">
         <v>40</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="J43" s="19"/>
+      <c r="C43" s="17"/>
+      <c r="D43" t="s">
+        <v>231</v>
+      </c>
+      <c r="E43" t="s">
+        <v>232</v>
+      </c>
+      <c r="I43" t="s">
+        <v>233</v>
+      </c>
       <c r="M43" t="s">
         <v>46</v>
       </c>
@@ -2561,18 +2541,15 @@
       <c r="B44">
         <v>41</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="16"/>
       <c r="D44" t="s">
-        <v>81</v>
+        <v>218</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="I44" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="M44" t="s">
         <v>44</v>
@@ -2585,15 +2562,18 @@
       <c r="B45">
         <v>42</v>
       </c>
-      <c r="C45" s="10"/>
+      <c r="C45" s="16"/>
       <c r="D45" t="s">
-        <v>81</v>
+        <v>234</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>221</v>
+      </c>
+      <c r="G45" t="s">
+        <v>209</v>
       </c>
       <c r="I45" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="M45" t="s">
         <v>45</v>
@@ -2606,15 +2586,18 @@
       <c r="B46">
         <v>43</v>
       </c>
-      <c r="C46" s="10"/>
+      <c r="C46" s="16"/>
       <c r="D46" t="s">
-        <v>81</v>
+        <v>210</v>
       </c>
       <c r="E46" t="s">
-        <v>42</v>
+        <v>214</v>
+      </c>
+      <c r="G46" t="s">
+        <v>222</v>
       </c>
       <c r="I46" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="M46" t="s">
         <v>47</v>
@@ -2630,18 +2613,18 @@
       <c r="B47">
         <v>44</v>
       </c>
-      <c r="C47" s="10"/>
+      <c r="C47" s="16"/>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>223</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>224</v>
       </c>
       <c r="G47" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I47" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="M47" t="s">
         <v>48</v>
@@ -2654,15 +2637,18 @@
       <c r="B48">
         <v>45</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="16"/>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
+        <v>212</v>
+      </c>
+      <c r="G48" t="s">
+        <v>225</v>
       </c>
       <c r="I48" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="M48" t="s">
         <v>49</v>
@@ -2675,15 +2661,18 @@
       <c r="B49">
         <v>46</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="16"/>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>217</v>
       </c>
       <c r="E49" t="s">
-        <v>213</v>
+        <v>216</v>
+      </c>
+      <c r="G49" t="s">
+        <v>148</v>
       </c>
       <c r="I49" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="M49" t="s">
         <v>55</v>
@@ -2696,15 +2685,15 @@
       <c r="B50">
         <v>47</v>
       </c>
-      <c r="C50" s="10"/>
+      <c r="C50" s="17"/>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>214</v>
+        <v>69</v>
       </c>
       <c r="I50" t="s">
-        <v>220</v>
+        <v>145</v>
       </c>
       <c r="M50" t="s">
         <v>50</v>
@@ -2720,15 +2709,15 @@
       <c r="B51">
         <v>48</v>
       </c>
-      <c r="C51" s="10"/>
+      <c r="C51" s="17"/>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E51" t="s">
-        <v>215</v>
+        <v>70</v>
       </c>
       <c r="I51" t="s">
-        <v>219</v>
+        <v>146</v>
       </c>
       <c r="M51" t="s">
         <v>127</v>
@@ -2741,15 +2730,15 @@
       <c r="B52">
         <v>49</v>
       </c>
-      <c r="C52" s="10"/>
+      <c r="C52" s="17"/>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E52" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="I52" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="M52" t="s">
         <v>51</v>
@@ -2762,15 +2751,15 @@
       <c r="B53">
         <v>50</v>
       </c>
-      <c r="C53" s="10"/>
+      <c r="C53" s="17"/>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="I53" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="M53" t="s">
         <v>53</v>
@@ -2786,22 +2775,16 @@
       <c r="B54">
         <v>51</v>
       </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="J54" s="19"/>
+      <c r="C54" s="17"/>
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" t="s">
+        <v>229</v>
+      </c>
+      <c r="I54" t="s">
+        <v>207</v>
+      </c>
       <c r="M54" t="s">
         <v>54</v>
       </c>
@@ -2814,20 +2797,6 @@
       <c r="B55">
         <v>52</v>
       </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="J55" s="19"/>
       <c r="M55" t="s">
         <v>65</v>
       </c>
@@ -2839,20 +2808,6 @@
       <c r="B56">
         <v>53</v>
       </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="J56" s="19"/>
       <c r="M56" t="s">
         <v>66</v>
       </c>
@@ -2862,23 +2817,10 @@
     </row>
     <row r="57" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="B57">
         <v>54</v>
-      </c>
-      <c r="C57" s="10"/>
-      <c r="D57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" t="s">
-        <v>55</v>
-      </c>
-      <c r="G57" t="s">
-        <v>234</v>
-      </c>
-      <c r="I57" t="s">
-        <v>227</v>
       </c>
       <c r="M57" t="s">
         <v>67</v>
@@ -2891,16 +2833,6 @@
       <c r="B58">
         <v>55</v>
       </c>
-      <c r="C58" s="10"/>
-      <c r="D58" t="s">
-        <v>78</v>
-      </c>
-      <c r="E58" t="s">
-        <v>50</v>
-      </c>
-      <c r="I58" t="s">
-        <v>228</v>
-      </c>
       <c r="M58" t="s">
         <v>68</v>
       </c>
@@ -2912,19 +2844,6 @@
       <c r="B59">
         <v>56</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59" t="s">
-        <v>51</v>
-      </c>
-      <c r="G59" t="s">
-        <v>233</v>
-      </c>
-      <c r="I59" t="s">
-        <v>229</v>
-      </c>
       <c r="M59" t="s">
         <v>69</v>
       </c>
@@ -2936,16 +2855,6 @@
       <c r="B60">
         <v>57</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" t="s">
-        <v>261</v>
-      </c>
-      <c r="E60" t="s">
-        <v>262</v>
-      </c>
-      <c r="I60" t="s">
-        <v>263</v>
-      </c>
       <c r="M60" t="s">
         <v>70</v>
       </c>
@@ -2960,16 +2869,6 @@
       <c r="B61">
         <v>58</v>
       </c>
-      <c r="C61" s="17"/>
-      <c r="D61" t="s">
-        <v>245</v>
-      </c>
-      <c r="E61" t="s">
-        <v>246</v>
-      </c>
-      <c r="I61" t="s">
-        <v>247</v>
-      </c>
       <c r="M61" t="s">
         <v>71</v>
       </c>
@@ -2981,19 +2880,6 @@
       <c r="B62">
         <v>59</v>
       </c>
-      <c r="C62" s="17"/>
-      <c r="D62" t="s">
-        <v>265</v>
-      </c>
-      <c r="E62" t="s">
-        <v>248</v>
-      </c>
-      <c r="G62" t="s">
-        <v>236</v>
-      </c>
-      <c r="I62" t="s">
-        <v>256</v>
-      </c>
       <c r="M62" t="s">
         <v>139</v>
       </c>
@@ -3005,19 +2891,6 @@
       <c r="B63">
         <v>60</v>
       </c>
-      <c r="C63" s="10"/>
-      <c r="D63" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" t="s">
-        <v>140</v>
-      </c>
-      <c r="G63" t="s">
-        <v>249</v>
-      </c>
-      <c r="I63" t="s">
-        <v>150</v>
-      </c>
       <c r="M63" t="s">
         <v>140</v>
       </c>
@@ -3029,19 +2902,6 @@
       <c r="B64">
         <v>61</v>
       </c>
-      <c r="C64" s="17"/>
-      <c r="D64" t="s">
-        <v>237</v>
-      </c>
-      <c r="E64" t="s">
-        <v>241</v>
-      </c>
-      <c r="G64" t="s">
-        <v>250</v>
-      </c>
-      <c r="I64" t="s">
-        <v>242</v>
-      </c>
       <c r="M64" t="s">
         <v>141</v>
       </c>
@@ -3053,19 +2913,6 @@
       <c r="B65">
         <v>62</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" t="s">
-        <v>251</v>
-      </c>
-      <c r="E65" t="s">
-        <v>252</v>
-      </c>
-      <c r="G65" t="s">
-        <v>254</v>
-      </c>
-      <c r="I65" t="s">
-        <v>257</v>
-      </c>
       <c r="M65" t="s">
         <v>144</v>
       </c>
@@ -3077,37 +2924,11 @@
       <c r="B66">
         <v>63</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" t="s">
-        <v>238</v>
-      </c>
-      <c r="E66" t="s">
-        <v>239</v>
-      </c>
-      <c r="G66" t="s">
-        <v>253</v>
-      </c>
-      <c r="I66" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="67" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B67">
         <v>64</v>
       </c>
-      <c r="C67" s="10"/>
-      <c r="D67" t="s">
-        <v>255</v>
-      </c>
-      <c r="E67" t="s">
-        <v>144</v>
-      </c>
-      <c r="G67" t="s">
-        <v>264</v>
-      </c>
-      <c r="I67" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="68" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
@@ -3116,49 +2937,16 @@
       <c r="B68">
         <v>65</v>
       </c>
-      <c r="C68" s="17"/>
-      <c r="D68" t="s">
-        <v>244</v>
-      </c>
-      <c r="E68" t="s">
-        <v>243</v>
-      </c>
-      <c r="G68" t="s">
-        <v>149</v>
-      </c>
-      <c r="I68" t="s">
-        <v>151</v>
-      </c>
     </row>
     <row r="69" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B69">
         <v>66</v>
       </c>
-      <c r="C69" s="18"/>
-      <c r="D69" t="s">
-        <v>79</v>
-      </c>
-      <c r="E69" t="s">
-        <v>69</v>
-      </c>
-      <c r="I69" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="70" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B70">
         <v>67</v>
       </c>
-      <c r="C70" s="18"/>
-      <c r="D70" t="s">
-        <v>79</v>
-      </c>
-      <c r="E70" t="s">
-        <v>70</v>
-      </c>
-      <c r="I70" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="71" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
@@ -3167,45 +2955,15 @@
       <c r="B71">
         <v>68</v>
       </c>
-      <c r="C71" s="18"/>
-      <c r="D71" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" t="s">
-        <v>71</v>
-      </c>
-      <c r="I71" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="72" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B72">
         <v>69</v>
       </c>
-      <c r="C72" s="17"/>
-      <c r="D72" t="s">
-        <v>125</v>
-      </c>
-      <c r="E72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I72" t="s">
-        <v>231</v>
-      </c>
     </row>
     <row r="73" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B73">
         <v>70</v>
-      </c>
-      <c r="C73" s="18"/>
-      <c r="D73" t="s">
-        <v>126</v>
-      </c>
-      <c r="E73" t="s">
-        <v>259</v>
-      </c>
-      <c r="I73" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>